<commit_message>
New Login tests are added.
</commit_message>
<xml_diff>
--- a/data/test plan.xlsx
+++ b/data/test plan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>ID: 1</t>
   </si>
@@ -40,9 +40,6 @@
     <t>danka@fakemail.com</t>
   </si>
   <si>
-    <t>Test case name: Log in with right credentials</t>
-  </si>
-  <si>
     <t>Data:</t>
   </si>
   <si>
@@ -89,6 +86,20 @@
   </si>
   <si>
     <t>Danka Radanovic</t>
+  </si>
+  <si>
+    <t>Test case name: Log in with real and wrong credenitals</t>
+  </si>
+  <si>
+    <t>There is 1 error
+Authentication failed.</t>
+  </si>
+  <si>
+    <t>No credentials</t>
+  </si>
+  <si>
+    <t>There is 1 error
+An email address required.</t>
   </si>
 </sst>
 </file>
@@ -141,7 +152,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -159,6 +170,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -462,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F15" sqref="F13:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,30 +488,31 @@
     <col min="2" max="2" width="46.7109375" customWidth="1"/>
     <col min="3" max="3" width="40.7109375" customWidth="1"/>
     <col min="4" max="4" width="23.140625" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="28.28515625" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
@@ -505,62 +520,66 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>18</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7">
         <v>123456789</v>
@@ -568,25 +587,31 @@
       <c r="E7">
         <v>111222333</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G8" t="s">
-        <v>23</v>
+      <c r="H8" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
address update test is added.
</commit_message>
<xml_diff>
--- a/data/test plan.xlsx
+++ b/data/test plan.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Log_in" sheetId="3" r:id="rId1"/>
+    <sheet name="My_address" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="43">
   <si>
     <t>ID: 1</t>
   </si>
@@ -100,6 +101,51 @@
   <si>
     <t>There is 1 error
 An email address required.</t>
+  </si>
+  <si>
+    <t>ID: 2</t>
+  </si>
+  <si>
+    <t>Test name: Update user address</t>
+  </si>
+  <si>
+    <t>DATA:</t>
+  </si>
+  <si>
+    <t>Bug report</t>
+  </si>
+  <si>
+    <t>Click on MyAddresses button</t>
+  </si>
+  <si>
+    <t>My address page is opened</t>
+  </si>
+  <si>
+    <t>Click on "update" button</t>
+  </si>
+  <si>
+    <t>Address fields page is opened</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>Input address2 in "Address (Line 2)" field</t>
+  </si>
+  <si>
+    <t>Novo naselje BB2</t>
+  </si>
+  <si>
+    <t>New address is inputed and visible</t>
+  </si>
+  <si>
+    <t>Click on "Save" button</t>
+  </si>
+  <si>
+    <t>Your addresses are listed below.</t>
+  </si>
+  <si>
+    <t>New address is saved</t>
   </si>
 </sst>
 </file>
@@ -152,7 +198,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -173,6 +219,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -476,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F13:F15"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,9 +541,10 @@
     <col min="6" max="6" width="20.85546875" customWidth="1"/>
     <col min="7" max="7" width="13.7109375" customWidth="1"/>
     <col min="8" max="8" width="11.42578125" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -511,8 +561,11 @@
       <c r="H1" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
@@ -529,12 +582,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -545,7 +598,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -556,7 +609,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>11</v>
       </c>
@@ -574,7 +627,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>12</v>
       </c>
@@ -591,7 +644,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>13</v>
       </c>
@@ -621,4 +674,173 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="45" customWidth="1"/>
+    <col min="3" max="3" width="37.140625" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7">
+        <v>123456789</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D6" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
log out test added.
</commit_message>
<xml_diff>
--- a/data/test plan.xlsx
+++ b/data/test plan.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Log_in" sheetId="3" r:id="rId1"/>
-    <sheet name="My_address" sheetId="4" r:id="rId2"/>
+    <sheet name="Log_out" sheetId="5" r:id="rId2"/>
+    <sheet name="My_address_update" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="48">
   <si>
     <t>ID: 1</t>
   </si>
@@ -99,10 +100,6 @@
     <t>No credentials</t>
   </si>
   <si>
-    <t>There is 1 error
-An email address required.</t>
-  </si>
-  <si>
     <t>ID: 2</t>
   </si>
   <si>
@@ -146,6 +143,24 @@
   </si>
   <si>
     <t>New address is saved</t>
+  </si>
+  <si>
+    <t>ID: 3</t>
+  </si>
+  <si>
+    <t>Test case name: Verify that user can log out</t>
+  </si>
+  <si>
+    <t>Click on "sign out" button on the upper right corner</t>
+  </si>
+  <si>
+    <t>user is logged out</t>
+  </si>
+  <si>
+    <t>Sign in</t>
+  </si>
+  <si>
+    <t>An email address required.</t>
   </si>
 </sst>
 </file>
@@ -198,7 +213,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -222,6 +237,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -527,8 +545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,7 +556,7 @@
     <col min="3" max="3" width="40.7109375" customWidth="1"/>
     <col min="4" max="4" width="23.140625" customWidth="1"/>
     <col min="5" max="5" width="28.28515625" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" customWidth="1"/>
+    <col min="6" max="6" width="28.85546875" customWidth="1"/>
     <col min="7" max="7" width="13.7109375" customWidth="1"/>
     <col min="8" max="8" width="11.42578125" customWidth="1"/>
     <col min="9" max="9" width="10.42578125" customWidth="1"/>
@@ -562,7 +580,7 @@
         <v>21</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -644,7 +662,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>13</v>
       </c>
@@ -658,7 +676,7 @@
         <v>25</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>6</v>
@@ -678,11 +696,142 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8" customWidth="1"/>
+    <col min="2" max="2" width="42.5703125" customWidth="1"/>
+    <col min="3" max="3" width="35" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7">
+        <v>123456789</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D6" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -697,10 +846,10 @@
   <sheetData>
     <row r="1" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>28</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>29</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>3</v>
@@ -709,7 +858,7 @@
         <v>21</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -720,7 +869,7 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -791,21 +940,21 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
         <v>32</v>
       </c>
-      <c r="C9" t="s">
-        <v>33</v>
-      </c>
       <c r="E9" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
         <v>34</v>
-      </c>
-      <c r="C10" t="s">
-        <v>35</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>6</v>
@@ -813,13 +962,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
         <v>37</v>
-      </c>
-      <c r="C11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" t="s">
-        <v>38</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>6</v>
@@ -827,13 +976,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" t="s">
         <v>40</v>
-      </c>
-      <c r="C12" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new tests added, for addresses and wishlist
</commit_message>
<xml_diff>
--- a/data/test plan.xlsx
+++ b/data/test plan.xlsx
@@ -4,19 +4,24 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Log_in" sheetId="3" r:id="rId1"/>
     <sheet name="Log_out" sheetId="5" r:id="rId2"/>
     <sheet name="My_address_update" sheetId="4" r:id="rId3"/>
+    <sheet name="Add_address" sheetId="6" r:id="rId4"/>
+    <sheet name="Remove_address " sheetId="7" r:id="rId5"/>
+    <sheet name="Edit_personal_info" sheetId="8" r:id="rId6"/>
+    <sheet name="Add_wish_list" sheetId="9" r:id="rId7"/>
+    <sheet name="Remove_wish_list" sheetId="10" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="97">
   <si>
     <t>ID: 1</t>
   </si>
@@ -85,9 +90,6 @@
   </si>
   <si>
     <t>assert</t>
-  </si>
-  <si>
-    <t>Danka Radanovic</t>
   </si>
   <si>
     <t>Test case name: Log in with real and wrong credenitals</t>
@@ -139,9 +141,6 @@
     <t>Click on "Save" button</t>
   </si>
   <si>
-    <t>Your addresses are listed below.</t>
-  </si>
-  <si>
     <t>New address is saved</t>
   </si>
   <si>
@@ -161,6 +160,159 @@
   </si>
   <si>
     <t>An email address required.</t>
+  </si>
+  <si>
+    <t>ID: 4</t>
+  </si>
+  <si>
+    <t>Test case name: Verify that user can add new address</t>
+  </si>
+  <si>
+    <t>Assert</t>
+  </si>
+  <si>
+    <t>Input adress in the adress field</t>
+  </si>
+  <si>
+    <t>Adress is inputed and visible</t>
+  </si>
+  <si>
+    <t>Input City in the city field</t>
+  </si>
+  <si>
+    <t>City is inputed and visible</t>
+  </si>
+  <si>
+    <t>Neka ulica</t>
+  </si>
+  <si>
+    <t>Novi Sad</t>
+  </si>
+  <si>
+    <t>Click on state dropdown bar</t>
+  </si>
+  <si>
+    <t>States are visible</t>
+  </si>
+  <si>
+    <t>Choose state</t>
+  </si>
+  <si>
+    <t>State is choosen and visible</t>
+  </si>
+  <si>
+    <t>Alabama</t>
+  </si>
+  <si>
+    <t>Input postcode in the postcode field</t>
+  </si>
+  <si>
+    <t>Input phone in the phone field</t>
+  </si>
+  <si>
+    <t>postcode is inputed and visible</t>
+  </si>
+  <si>
+    <t>phone is inputed and visible</t>
+  </si>
+  <si>
+    <t>Input alias address</t>
+  </si>
+  <si>
+    <t>address is added and visible</t>
+  </si>
+  <si>
+    <t>Neka adresa</t>
+  </si>
+  <si>
+    <t>NEKA ADRESA</t>
+  </si>
+  <si>
+    <t>Click on the "Save" button</t>
+  </si>
+  <si>
+    <t>new address is added</t>
+  </si>
+  <si>
+    <t>ID: 5</t>
+  </si>
+  <si>
+    <t>Test case name: Verify that user can delete the address</t>
+  </si>
+  <si>
+    <t>Click on "delete" button</t>
+  </si>
+  <si>
+    <t>ID: 6</t>
+  </si>
+  <si>
+    <t>Test case name: Verify that user can change personal info</t>
+  </si>
+  <si>
+    <t>Click on "my personal info" button</t>
+  </si>
+  <si>
+    <t>Page with personal info is opened</t>
+  </si>
+  <si>
+    <t>Input lastname in the last name field</t>
+  </si>
+  <si>
+    <t>lastname is inputed and visible</t>
+  </si>
+  <si>
+    <t>Input current password</t>
+  </si>
+  <si>
+    <t>password is inputed</t>
+  </si>
+  <si>
+    <t>Nesto</t>
+  </si>
+  <si>
+    <t>Click on Save button</t>
+  </si>
+  <si>
+    <t>edit is successfully saved</t>
+  </si>
+  <si>
+    <t>Your personal information has been successfully updated.</t>
+  </si>
+  <si>
+    <t>Sign out</t>
+  </si>
+  <si>
+    <t>ID: 7</t>
+  </si>
+  <si>
+    <t>Test case name: verify that user can add new wishlist</t>
+  </si>
+  <si>
+    <t>Click on "My Wishlists" button</t>
+  </si>
+  <si>
+    <t>Page with wishlists is opened</t>
+  </si>
+  <si>
+    <t>Inout name in the new wishlist name field</t>
+  </si>
+  <si>
+    <t>Name is inputed and visible</t>
+  </si>
+  <si>
+    <t>Neka lista</t>
+  </si>
+  <si>
+    <t>Wishlist is saved and visible</t>
+  </si>
+  <si>
+    <t>ID: 8</t>
+  </si>
+  <si>
+    <t>Test case name: Verify  that user can remove wishlist</t>
+  </si>
+  <si>
+    <t>Click on x button</t>
   </si>
 </sst>
 </file>
@@ -213,7 +365,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -240,6 +392,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -545,8 +700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,10 +722,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C1" s="3"/>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>8</v>
       </c>
       <c r="G1" s="4" t="s">
@@ -580,7 +735,7 @@
         <v>21</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -597,7 +752,7 @@
         <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -670,13 +825,13 @@
         <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>85</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>6</v>
@@ -691,15 +846,16 @@
     <hyperlink ref="E6" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,20 +865,28 @@
     <col min="3" max="3" width="35" customWidth="1"/>
     <col min="4" max="4" width="25.28515625" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E1" s="10" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
@@ -730,17 +894,17 @@
         <v>2</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -751,7 +915,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -762,7 +926,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>11</v>
       </c>
@@ -776,7 +940,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>12</v>
       </c>
@@ -790,7 +954,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>13</v>
       </c>
@@ -798,24 +962,27 @@
         <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>85</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" t="s">
         <v>44</v>
       </c>
-      <c r="C9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" t="s">
-        <v>46</v>
-      </c>
       <c r="E9" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="F9" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -831,7 +998,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -846,19 +1015,19 @@
   <sheetData>
     <row r="1" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="9" t="s">
-        <v>30</v>
+      <c r="G1" s="7" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -869,7 +1038,7 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -940,21 +1109,21 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" t="s">
-        <v>32</v>
-      </c>
       <c r="E9" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s">
         <v>33</v>
-      </c>
-      <c r="C10" t="s">
-        <v>34</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>6</v>
@@ -962,13 +1131,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" t="s">
         <v>36</v>
-      </c>
-      <c r="C11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" t="s">
-        <v>37</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>6</v>
@@ -976,13 +1145,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" t="s">
         <v>39</v>
       </c>
-      <c r="C12" t="s">
-        <v>41</v>
-      </c>
       <c r="D12" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -992,4 +1161,963 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.42578125" customWidth="1"/>
+    <col min="2" max="2" width="36.28515625" customWidth="1"/>
+    <col min="3" max="3" width="35" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7">
+        <v>123456789</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14">
+        <v>21000</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15">
+        <v>601234567</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" t="s">
+        <v>66</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D6" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="33" customWidth="1"/>
+    <col min="3" max="3" width="31.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7">
+        <v>123456789</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14">
+        <v>21000</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15">
+        <v>601234567</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" t="s">
+        <v>66</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D6" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="34.85546875" customWidth="1"/>
+    <col min="3" max="3" width="34.28515625" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="9"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7">
+        <v>123456789</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11">
+        <v>123456789</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D6" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" customWidth="1"/>
+    <col min="2" max="2" width="46.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.85546875" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7">
+        <v>123456789</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" t="s">
+        <v>89</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" t="s">
+        <v>91</v>
+      </c>
+      <c r="D10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
+        <v>93</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D6" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" customWidth="1"/>
+    <col min="2" max="2" width="37.7109375" customWidth="1"/>
+    <col min="3" max="3" width="35.140625" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7">
+        <v>123456789</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" t="s">
+        <v>91</v>
+      </c>
+      <c r="D10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D6" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>